<commit_message>
Update Pertanggal 9 November 2023 14:17 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Others/COA Auto Journal.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Others/COA Auto Journal.xlsx
@@ -1,21 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Debit Note (3)" sheetId="3" r:id="rId1"/>
+    <sheet name="Debit Note (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="Debit Note" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
+  <si>
+    <t>Pembelian Barang</t>
+  </si>
+  <si>
+    <t>Utang Usaha</t>
+  </si>
+  <si>
+    <t>Persediaan</t>
+  </si>
+  <si>
+    <t>Kas/Bank</t>
+  </si>
+  <si>
+    <t>ACTIVA</t>
+  </si>
+  <si>
+    <t>PASIVA</t>
+  </si>
+  <si>
+    <t>TANGGAL</t>
+  </si>
+  <si>
+    <t>URAIAN</t>
+  </si>
+  <si>
+    <t>COA</t>
+  </si>
+  <si>
+    <t>NILAI</t>
+  </si>
+  <si>
+    <t>DEBET</t>
+  </si>
+  <si>
+    <t>KREDIT</t>
+  </si>
+  <si>
+    <t>BUKU BESAR</t>
+  </si>
+  <si>
+    <t>JURNAL</t>
+  </si>
+  <si>
+    <t>Penerimaan Kas/Bank atas Retur Barang</t>
+  </si>
+  <si>
+    <t>Retur Barang</t>
+  </si>
+  <si>
+    <t>Pembayaran Invoice Pembelian</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +85,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -40,18 +146,179 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +365,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +400,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +608,790 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="11" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="I2" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="I3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
+        <v>44928</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="I5" s="12">
+        <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:K12" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" ref="I6:I12" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>44941</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="I7" s="10">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
+        <v>-1000000</v>
+      </c>
+      <c r="K8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
+        <v>44946</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <v>200000</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="I9" s="10">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="0"/>
+        <v>-1000000</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" si="0"/>
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17">
+        <v>200000</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
+        <v>800000</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="0"/>
+        <v>-1000000</v>
+      </c>
+      <c r="K10" s="10">
+        <f t="shared" si="0"/>
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="9">
+        <v>44951</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="14">
+        <v>200000</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
+        <v>800000</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="0"/>
+        <v>-800000</v>
+      </c>
+      <c r="K11" s="10">
+        <f t="shared" si="0"/>
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17">
+        <v>200000</v>
+      </c>
+      <c r="I12" s="11">
+        <f t="shared" si="1"/>
+        <v>800000</v>
+      </c>
+      <c r="J12" s="11">
+        <f t="shared" si="0"/>
+        <v>-800000</v>
+      </c>
+      <c r="K12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="11" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="I2" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="I3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
+        <v>44928</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="I5" s="12">
+        <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:K10" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" ref="I6:I10" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>44936</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>200000</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="I7" s="10">
+        <f t="shared" ref="I7:I10" si="2">(IF(ISNUMBER(I6), I6, 0) + IF(EXACT(I$4, $D7), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E7), IF(EXACT(I$4, $F7), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G7), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" ref="J7:J10" si="3">(IF(ISNUMBER(J6), J6, 0) + IF(EXACT(J$4, $D7), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E7), IF(EXACT(J$4, $F7), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G7), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" ref="K7:K10" si="4">(IF(ISNUMBER(K6), K6, 0) + IF(EXACT(K$4, $D7), ((IF(EXACT(K$3, "ACTIVA"), 1, -1)) * $E7), IF(EXACT(K$4, $F7), ((IF(EXACT(K$3, "ACTIVA"), 1, -1)) * -$G7), 0)))</f>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="17">
+        <v>200000</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="2"/>
+        <v>800000</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <f t="shared" si="4"/>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
+        <v>44941</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14">
+        <v>800000</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="I9" s="10">
+        <f t="shared" si="2"/>
+        <v>800000</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="17">
+        <v>800000</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="2"/>
+        <v>800000</v>
+      </c>
+      <c r="J10" s="11">
+        <f t="shared" si="3"/>
+        <v>-800000</v>
+      </c>
+      <c r="K10" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="11" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="I2" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
+    </row>
+    <row r="3" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="I3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
+        <v>44928</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="I5" s="12">
+        <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:K8" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" ref="I6:I8" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>44941</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="I7" s="10">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="J8" s="11">
+        <f t="shared" si="0"/>
+        <v>-1000000</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pertanggal 28 November 2023 08:48 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Others/COA Auto Journal.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Others/COA Auto Journal.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Debit Note (3)" sheetId="3" r:id="rId1"/>
-    <sheet name="Debit Note (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Debit Note" sheetId="1" r:id="rId3"/>
+    <sheet name="ARF Belum dibayar yang Disettle" sheetId="5" r:id="rId1"/>
+    <sheet name="ARF dengan RPC" sheetId="4" r:id="rId2"/>
+    <sheet name="Debit Note (3)" sheetId="3" r:id="rId3"/>
+    <sheet name="Debit Note (2)" sheetId="2" r:id="rId4"/>
+    <sheet name="Debit Note" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="25">
   <si>
     <t>Pembelian Barang</t>
   </si>
@@ -67,6 +69,30 @@
   </si>
   <si>
     <t>Pembayaran Invoice Pembelian</t>
+  </si>
+  <si>
+    <t>Pembayaran Advance</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Pertanggung Jawaban Advance</t>
+  </si>
+  <si>
+    <t>Biaya</t>
+  </si>
+  <si>
+    <t>Piutang Karyawan</t>
+  </si>
+  <si>
+    <t>Uang Muka Karyawan</t>
+  </si>
+  <si>
+    <t>Pengembalian Sisa Uang ke Perusahaan</t>
+  </si>
+  <si>
+    <t>Pembayaran Uang ke Karyawan</t>
   </si>
 </sst>
 </file>
@@ -75,7 +101,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -239,27 +265,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -271,31 +288,34 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,6 +324,36 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,6 +659,565 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" s="18" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="I3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="19">
+        <v>44941</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1500000</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="I5" s="9">
+        <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:L5" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" si="0"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="19"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1500000</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" ref="I6:L8" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>-1500000</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="1"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="19">
+        <v>44943</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1500000</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="1"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="19"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1500000</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>-1500000</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="1"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" s="18" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="I3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="19">
+        <v>44928</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2000000</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="I5" s="9">
+        <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:K6" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>2000000</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" ref="L5" si="1">(IF(ISNUMBER(L4), L4, 0) + IF(EXACT(L$4, $D5), ((IF(EXACT(L$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(L$4, $F5), ((IF(EXACT(L$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="19"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" ref="I6:L11" si="2">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
+        <v>-2000000</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="19">
+        <v>44941</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1500000</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="7">
+        <f t="shared" si="2"/>
+        <v>-2000000</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="19"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="28">
+        <v>500000</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
+      <c r="I8" s="7">
+        <f t="shared" si="2"/>
+        <v>-2000000</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="2"/>
+        <v>-500000</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="19"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="2"/>
+        <v>-2000000</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="2"/>
+        <v>-500000</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="19">
+        <v>44943</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="11">
+        <v>500000</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="I10" s="7">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="2"/>
+        <v>-500000</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="19"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="13">
+        <v>500000</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <f t="shared" si="2"/>
+        <v>-1500000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -629,281 +1238,287 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:11" s="18" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="I2" s="24" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="26"/>
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="9">
+      <c r="B5" s="19">
         <v>44928</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14">
-        <v>1000000</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="I5" s="12">
+      <c r="E5" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="I5" s="9">
         <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
         <v>1000000</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <f t="shared" ref="J5:K12" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
         <v>0</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="17">
-        <v>1000000</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="G6" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" ref="I6:I12" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
         <v>1000000</v>
       </c>
-      <c r="J6" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="9">
+      <c r="B7" s="19">
         <v>44941</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="14">
-        <v>1000000</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="I7" s="10">
+      <c r="E7" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="7">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="J7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="16" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="17">
-        <v>1000000</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="G8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="7">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="7">
         <f t="shared" si="0"/>
         <v>-1000000</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="9">
+      <c r="B9" s="19">
         <v>44946</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <v>200000</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="I9" s="10">
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="I9" s="7">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="7">
         <f t="shared" si="0"/>
         <v>-1000000</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="7">
         <f t="shared" si="0"/>
         <v>-200000</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="16" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="13">
         <v>200000</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <f t="shared" si="1"/>
         <v>800000</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
         <v>-1000000</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="7">
         <f t="shared" si="0"/>
         <v>-200000</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="9">
+      <c r="B11" s="19">
         <v>44951</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>200000</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
-      <c r="I11" s="10">
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="I11" s="7">
         <f t="shared" si="1"/>
         <v>800000</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="7">
         <f t="shared" si="0"/>
         <v>-800000</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="7">
         <f t="shared" si="0"/>
         <v>-200000</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="16" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="13">
         <v>200000</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="8">
         <f t="shared" si="1"/>
         <v>800000</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="8">
         <f t="shared" si="0"/>
         <v>-800000</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B5:B6"/>
@@ -912,19 +1527,13 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K10"/>
   <sheetViews>
@@ -946,253 +1555,253 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:11" s="18" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="I2" s="24" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="26"/>
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="9">
+      <c r="B5" s="19">
         <v>44928</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14">
-        <v>1000000</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="I5" s="12">
+      <c r="E5" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="I5" s="9">
         <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
         <v>1000000</v>
       </c>
-      <c r="J5" s="12">
-        <f t="shared" ref="J5:K10" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="12">
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:K6" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="17">
-        <v>1000000</v>
-      </c>
-      <c r="I6" s="10">
-        <f t="shared" ref="I6:I10" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
-        <v>1000000</v>
-      </c>
-      <c r="J6" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="G6" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" ref="I6" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
+        <v>1000000</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="9">
+      <c r="B7" s="19">
         <v>44936</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="11">
         <v>200000</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="I7" s="10">
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="7">
         <f t="shared" ref="I7:I10" si="2">(IF(ISNUMBER(I6), I6, 0) + IF(EXACT(I$4, $D7), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E7), IF(EXACT(I$4, $F7), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G7), 0)))</f>
         <v>1000000</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <f t="shared" ref="J7:J10" si="3">(IF(ISNUMBER(J6), J6, 0) + IF(EXACT(J$4, $D7), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E7), IF(EXACT(J$4, $F7), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G7), 0)))</f>
         <v>0</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <f t="shared" ref="K7:K10" si="4">(IF(ISNUMBER(K6), K6, 0) + IF(EXACT(K$4, $D7), ((IF(EXACT(K$3, "ACTIVA"), 1, -1)) * $E7), IF(EXACT(K$4, $F7), ((IF(EXACT(K$3, "ACTIVA"), 1, -1)) * -$G7), 0)))</f>
         <v>800000</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="16" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="13">
         <v>200000</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <f t="shared" si="2"/>
         <v>800000</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="7">
         <f t="shared" si="4"/>
         <v>800000</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="9">
+      <c r="B9" s="19">
         <v>44941</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <v>800000</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="I9" s="10">
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="I9" s="7">
         <f t="shared" si="2"/>
         <v>800000</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="16" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="13">
         <v>800000</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="8">
         <f t="shared" si="2"/>
         <v>800000</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="8">
         <f t="shared" si="3"/>
         <v>-800000</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1209,171 +1818,171 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:11" s="18" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="I2" s="24" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="I3" s="8" t="s">
+      <c r="G3" s="26"/>
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="9">
+      <c r="B5" s="19">
         <v>44928</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14">
-        <v>1000000</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
-      <c r="I5" s="12">
+      <c r="E5" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="I5" s="9">
         <f>(IF(ISNUMBER(I4), I4, 0) + IF(EXACT(I$4, $D5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(I$4, $F5), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
         <v>1000000</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <f t="shared" ref="J5:K8" si="0">(IF(ISNUMBER(J4), J4, 0) + IF(EXACT(J$4, $D5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * $E5), IF(EXACT(J$4, $F5), ((IF(EXACT(J$3, "ACTIVA"), 1, -1)) * -$G5), 0)))</f>
         <v>0</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="16" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="17">
-        <v>1000000</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="G6" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" ref="I6:I8" si="1">(IF(ISNUMBER(I5), I5, 0) + IF(EXACT(I$4, $D6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * $E6), IF(EXACT(I$4, $F6), ((IF(EXACT(I$3, "ACTIVA"), 1, -1)) * -$G6), 0)))</f>
         <v>1000000</v>
       </c>
-      <c r="J6" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="9">
+      <c r="B7" s="19">
         <v>44941</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="14">
-        <v>1000000</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="I7" s="10">
+      <c r="E7" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="7">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="J7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="16" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="17">
-        <v>1000000</v>
-      </c>
-      <c r="I8" s="11">
+      <c r="G8" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="8">
         <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="8">
         <f t="shared" si="0"/>
         <v>-1000000</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>